<commit_message>
Arreglos código de proyecto
</commit_message>
<xml_diff>
--- a/RespuestasTest.xlsx
+++ b/RespuestasTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFORMATICA\3ER SEMESTRE\INF-134 (ESTADÍSTICA II)\PROY ESTADÍSTICA II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFORMATICA\3ER SEMESTRE\INF-134 (ESTADÍSTICA II)\Proyecto-Estad-stica-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ECE412-15B9-4B3A-96F2-646A77DBBBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED72B0E-A1F4-4E60-8099-690ACBECE02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -944,8 +944,8 @@
   <dimension ref="A1:T62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>